<commit_message>
updated review protocol #3
</commit_message>
<xml_diff>
--- a/doc/SprintReviewProtocols/Sprint_Review_Protocol#3.xlsx
+++ b/doc/SprintReviewProtocols/Sprint_Review_Protocol#3.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="15395" windowHeight="13595"/>
+    <workbookView windowWidth="15395" windowHeight="12911"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -141,12 +141,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_-&quot;€&quot;\ * #,##0.00_-;\-&quot;€&quot;\ * #,##0.00_-;_-&quot;€&quot;\ * \-??_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="_-&quot;€&quot;\ * #,##0_-;\-&quot;€&quot;\ * #,##0_-;_-&quot;€&quot;\ * \-_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="_-&quot;€&quot;\ * #,##0_-;\-&quot;€&quot;\ * #,##0_-;_-&quot;€&quot;\ * \-_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="_-&quot;€&quot;\ * #,##0.00_-;\-&quot;€&quot;\ * #,##0.00_-;_-&quot;€&quot;\ * \-??_-;_-@_-"/>
   </numFmts>
-  <fonts count="25">
+  <fonts count="24">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -199,9 +199,9 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -223,14 +223,6 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -253,6 +245,14 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
@@ -276,22 +276,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -320,22 +314,21 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="37">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -368,25 +361,169 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -398,157 +535,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -754,6 +741,17 @@
     <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
@@ -799,162 +797,151 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="16" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="16" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="24" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1340,7 +1327,7 @@
   <dimension ref="A1:I32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
@@ -1555,10 +1542,12 @@
       <c r="C16" s="20">
         <v>0.25</v>
       </c>
-      <c r="D16" s="20"/>
+      <c r="D16" s="20">
+        <v>0.25</v>
+      </c>
       <c r="E16" s="21">
         <f>D16-C16</f>
-        <v>-0.25</v>
+        <v>0</v>
       </c>
       <c r="F16" s="22"/>
       <c r="G16" s="23"/>
@@ -1571,11 +1560,15 @@
       <c r="B17" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="C17" s="20"/>
-      <c r="D17" s="20"/>
+      <c r="C17" s="20">
+        <v>1.5</v>
+      </c>
+      <c r="D17" s="20">
+        <v>1</v>
+      </c>
       <c r="E17" s="21">
-        <f t="shared" ref="E17:E25" si="0">D17-C17</f>
-        <v>0</v>
+        <f t="shared" ref="E17:E26" si="0">D17-C17</f>
+        <v>-0.5</v>
       </c>
       <c r="F17" s="22"/>
       <c r="G17" s="23"/>
@@ -1588,8 +1581,12 @@
       <c r="B18" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="C18" s="20"/>
-      <c r="D18" s="20"/>
+      <c r="C18" s="20">
+        <v>2</v>
+      </c>
+      <c r="D18" s="20">
+        <v>2</v>
+      </c>
       <c r="E18" s="21">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1626,14 +1623,20 @@
       <c r="B20" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="C20" s="20"/>
-      <c r="D20" s="20"/>
+      <c r="C20" s="20">
+        <v>2.5</v>
+      </c>
+      <c r="D20" s="20">
+        <v>0</v>
+      </c>
       <c r="E20" s="21">
         <f t="shared" si="0"/>
+        <v>-2.5</v>
+      </c>
+      <c r="F20" s="22"/>
+      <c r="G20" s="23">
         <v>0</v>
       </c>
-      <c r="F20" s="22"/>
-      <c r="G20" s="23"/>
       <c r="H20" s="20"/>
     </row>
     <row r="21" spans="1:8">
@@ -1715,7 +1718,7 @@
         <v>0.5</v>
       </c>
       <c r="E24" s="21">
-        <f>D24-C24</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F24" s="22"/>
@@ -1736,7 +1739,7 @@
         <v>1</v>
       </c>
       <c r="E25" s="21">
-        <f>D25-C25</f>
+        <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
       <c r="F25" s="22"/>
@@ -1757,7 +1760,7 @@
         <v>0.5</v>
       </c>
       <c r="E26" s="21">
-        <f>D26-C26</f>
+        <f t="shared" si="0"/>
         <v>-0.5</v>
       </c>
       <c r="F26" s="22"/>
@@ -1774,7 +1777,7 @@
       <c r="D27" s="24"/>
       <c r="E27" s="24">
         <f>SUM(E16:E26)</f>
-        <v>-2.5</v>
+        <v>-5.25</v>
       </c>
       <c r="F27" s="24">
         <f>COUNT(F16:F26)</f>
@@ -1782,7 +1785,7 @@
       </c>
       <c r="G27" s="24">
         <f>COUNT(G16:G26)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H27" s="24"/>
     </row>

</xml_diff>

<commit_message>
added/adapted review protocol and screenshot email projectkitchen
</commit_message>
<xml_diff>
--- a/doc/SprintReviewProtocols/Sprint_Review_Protocol#3.xlsx
+++ b/doc/SprintReviewProtocols/Sprint_Review_Protocol#3.xlsx
@@ -141,10 +141,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_-&quot;€&quot;\ * #,##0.00_-;\-&quot;€&quot;\ * #,##0.00_-;_-&quot;€&quot;\ * \-??_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="176" formatCode="_-&quot;€&quot;\ * #,##0_-;\-&quot;€&quot;\ * #,##0_-;_-&quot;€&quot;\ * \-_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="_-&quot;€&quot;\ * #,##0.00_-;\-&quot;€&quot;\ * #,##0.00_-;_-&quot;€&quot;\ * \-??_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="_-&quot;€&quot;\ * #,##0_-;\-&quot;€&quot;\ * #,##0_-;_-&quot;€&quot;\ * \-_-;_-@_-"/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -199,7 +199,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -221,6 +221,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
@@ -237,8 +244,63 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -252,68 +314,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="Calibri"/>
@@ -361,73 +361,169 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -439,103 +535,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -697,6 +697,21 @@
         <color auto="1"/>
       </top>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -741,35 +756,9 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -797,10 +786,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -809,40 +809,40 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="16" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="17" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -851,40 +851,40 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="19" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="19" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -893,55 +893,55 @@
     <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1327,7 +1327,7 @@
   <dimension ref="A1:I32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
@@ -1549,7 +1549,9 @@
         <f>D16-C16</f>
         <v>0</v>
       </c>
-      <c r="F16" s="22"/>
+      <c r="F16" s="22">
+        <v>1</v>
+      </c>
       <c r="G16" s="23"/>
       <c r="H16" s="20"/>
     </row>
@@ -1570,7 +1572,9 @@
         <f t="shared" ref="E17:E26" si="0">D17-C17</f>
         <v>-0.5</v>
       </c>
-      <c r="F17" s="22"/>
+      <c r="F17" s="22">
+        <v>1</v>
+      </c>
       <c r="G17" s="23"/>
       <c r="H17" s="20"/>
     </row>
@@ -1591,7 +1595,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F18" s="22"/>
+      <c r="F18" s="22">
+        <v>1</v>
+      </c>
       <c r="G18" s="23"/>
       <c r="H18" s="20"/>
     </row>
@@ -1612,7 +1618,9 @@
         <f t="shared" si="0"/>
         <v>-0.25</v>
       </c>
-      <c r="F19" s="22"/>
+      <c r="F19" s="22">
+        <v>1</v>
+      </c>
       <c r="G19" s="23"/>
       <c r="H19" s="20"/>
     </row>
@@ -1656,7 +1664,9 @@
         <f t="shared" si="0"/>
         <v>-0.5</v>
       </c>
-      <c r="F21" s="22"/>
+      <c r="F21" s="22">
+        <v>1</v>
+      </c>
       <c r="G21" s="23"/>
       <c r="H21" s="20"/>
     </row>
@@ -1700,7 +1710,9 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="F23" s="22"/>
+      <c r="F23" s="22">
+        <v>1</v>
+      </c>
       <c r="G23" s="23"/>
       <c r="H23" s="20"/>
     </row>
@@ -1721,7 +1733,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F24" s="22"/>
+      <c r="F24" s="22">
+        <v>1</v>
+      </c>
       <c r="G24" s="23"/>
       <c r="H24" s="20"/>
     </row>
@@ -1742,7 +1756,9 @@
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="F25" s="22"/>
+      <c r="F25" s="22">
+        <v>1</v>
+      </c>
       <c r="G25" s="23"/>
       <c r="H25" s="20"/>
     </row>
@@ -1763,7 +1779,9 @@
         <f t="shared" si="0"/>
         <v>-0.5</v>
       </c>
-      <c r="F26" s="22"/>
+      <c r="F26" s="22">
+        <v>1</v>
+      </c>
       <c r="G26" s="23"/>
       <c r="H26" s="20"/>
     </row>
@@ -1781,7 +1799,7 @@
       </c>
       <c r="F27" s="24">
         <f>COUNT(F16:F26)</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="G27" s="24">
         <f>COUNT(G16:G26)</f>

</xml_diff>